<commit_message>
Update feedback and make GDD v2
</commit_message>
<xml_diff>
--- a/AIE Year 2/Psychology and Economies/Greco Feudal Docs/Greco Feudal Feedback.xlsx
+++ b/AIE Year 2/Psychology and Economies/Greco Feudal Docs/Greco Feudal Feedback.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s200479\Repos\Williams_Backpack\AIE Year 2\Psychology and Economies\Greco Feudal Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E426A754-CA30-47B0-ADBE-DE1E9CAF14AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84ECC472-B53B-4EB8-BE20-3205E996B95B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4095" yWindow="2415" windowWidth="21600" windowHeight="11385" xr2:uid="{46E08FCF-ADDE-46E4-8514-CE4E35947774}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{46E08FCF-ADDE-46E4-8514-CE4E35947774}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -57,7 +57,33 @@
     <t>• You want to identify your game's moral argument or theme ASAP. I'm still not sure what the message of the game is and hence the direction/vision.</t>
   </si>
   <si>
-    <t>Flesh out the theme and message I'm trying to tell with the game, and fit in the gameplay.</t>
+    <t>10 Pager v1</t>
+  </si>
+  <si>
+    <t>•With the Target Market, I'd like to see at least 5 profiles from social media where connections have been made and characteristics identified. You have identified the characteristics but I don't know where you got the info from.
+•I'd also like to see wire-frame mockups for the UI and mechanics.</t>
+  </si>
+  <si>
+    <t>Elric</t>
+  </si>
+  <si>
+    <t>•Flesh out the theme and message I'm trying to tell with the game, and fit in the gameplay.</t>
+  </si>
+  <si>
+    <t>•What platform is it on? (list in overview somewhere).
+•Maybe the japanese culture could be more of a flourish or emphasis rather than a core part of the aesthetic, so as not to confuse the player? OR make that blend of cultures a lot clearer in the story.
+•Images worked really well to explain the look and environmental mechanics!
+•What is the age rating.
+•Clarify if each combat mechanic is consistent for NPCs and PC enemy or if some of them are only intended for one or the other.</t>
+  </si>
+  <si>
+    <t>•Add information such as platform and age rating.
+•Explain exactly how the culture blend will be used and what it adds to the game.
+•Add more info for mechanics</t>
+  </si>
+  <si>
+    <t>•Add profiles for target market and description of relationship.
+•Finish wireframe.</t>
   </si>
 </sst>
 </file>
@@ -427,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F97EEB4C-CC96-4439-AA7F-5E0D5AD544D4}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,7 +491,35 @@
         <v>6</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>